<commit_message>
fix the weight summary lable
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/JLFHLZN.xlsx
+++ b/invoice_gen/TEMPLATE/JLFHLZN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\automate invoice\invoice_gen\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\inv_pkl_contract_creation\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3391CA74-92CC-4513-9A4C-2F4298485BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90700952-99EA-4D10-A66C-2E8A3E73A9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="10" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Packing list" sheetId="12" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$1:$F$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$32</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Packing list'!$A$1:$I$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$1:$F$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Packing list'!$A$1:$I$29</definedName>
   </definedNames>
   <calcPr calcId="191029" fullPrecision="0"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="84">
   <si>
     <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t xml:space="preserve">NO.:  </t>
-  </si>
-  <si>
-    <t>JLFHLZN25005</t>
   </si>
   <si>
     <t xml:space="preserve">DATE: </t>
@@ -230,9 +227,6 @@
     <t>Ref No:</t>
   </si>
   <si>
-    <t>CLF2025-149</t>
-  </si>
-  <si>
     <t>EXPORTER:</t>
   </si>
   <si>
@@ -413,10 +407,13 @@
     </r>
   </si>
   <si>
-    <t>JFNO</t>
-  </si>
-  <si>
     <t>JFTIME</t>
+  </si>
+  <si>
+    <t>JFREF</t>
+  </si>
+  <si>
+    <t>JFINV</t>
   </si>
 </sst>
 </file>
@@ -426,12 +423,12 @@
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
-    <numFmt numFmtId="167" formatCode="d\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0.00_ ;_-&quot;$&quot;* \-#,##0.00\ ;_-&quot;$&quot;* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="169" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="170" formatCode="0.0_);[Red]\(0.0\)"/>
+    <numFmt numFmtId="166" formatCode="d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0.00_ ;_-&quot;$&quot;* \-#,##0.00\ ;_-&quot;$&quot;* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="168" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="169" formatCode="0.0_);[Red]\(0.0\)"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,12 +497,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Book Antiqua"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Book Antiqua"/>
@@ -540,12 +531,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
@@ -680,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -706,33 +691,31 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -748,28 +731,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -778,16 +760,16 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -796,39 +778,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -837,16 +819,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -867,7 +849,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1011,13 +993,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>796925</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1210310</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>5715</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1055,13 +1037,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1104,13 +1086,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>93980</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>647065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>92075</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>350520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1148,13 +1130,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>64135</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>552450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>746125</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>186055</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1451,461 +1433,461 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="41" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="41" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="41" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" style="41" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="41"/>
-    <col min="8" max="16384" width="7.5703125" style="41"/>
+    <col min="1" max="1" width="22.7109375" style="38" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="38" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="38" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" style="38" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="38" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="38"/>
+    <col min="8" max="16384" width="7.5703125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="40" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:8" s="37" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-    </row>
-    <row r="2" spans="1:8" s="40" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="65" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+    </row>
+    <row r="2" spans="1:8" s="37" customFormat="1" ht="24" customHeight="1">
+      <c r="A2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-    </row>
-    <row r="3" spans="1:8" s="40" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A3" s="66" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+    </row>
+    <row r="3" spans="1:8" s="37" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A3" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-    </row>
-    <row r="4" spans="1:8" s="40" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A4" s="65" t="s">
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+    </row>
+    <row r="4" spans="1:8" s="37" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A4" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-    </row>
-    <row r="5" spans="1:8" s="40" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A5" s="67" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+    </row>
+    <row r="5" spans="1:8" s="37" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A5" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:8" ht="27" customHeight="1">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45" t="s">
+      <c r="A7" s="42"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45" t="s">
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="45"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="46" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45" t="s">
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="45" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="42"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="42"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+    </row>
+    <row r="17" spans="1:8" ht="27.95" customHeight="1">
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="45"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="46"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+    </row>
+    <row r="27" spans="1:8" ht="18.75">
+      <c r="A27" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="48"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="45"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="45"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-    </row>
-    <row r="17" spans="1:8" ht="27.95" customHeight="1">
-      <c r="A17" s="59"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="48"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="49"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="45"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-    </row>
-    <row r="27" spans="1:8" ht="18.75">
-      <c r="A27" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="51"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="45" t="s">
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+    </row>
+    <row r="29" spans="1:8" ht="26.1" customHeight="1">
+      <c r="A29" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B29" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+    </row>
+    <row r="31" spans="1:8" ht="27" customHeight="1">
+      <c r="A31" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="52"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75">
+      <c r="A32" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="52"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75">
+      <c r="A33" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="52"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75">
+      <c r="A34" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="52"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="42"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-    </row>
-    <row r="29" spans="1:8" ht="26.1" customHeight="1">
-      <c r="A29" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="63" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-    </row>
-    <row r="31" spans="1:8" ht="27" customHeight="1">
-      <c r="A31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="55"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75">
-      <c r="A32" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="55"/>
-    </row>
-    <row r="33" spans="1:8" ht="15.75">
-      <c r="A33" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="55"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75">
-      <c r="A34" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="55"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="45"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="45" t="s">
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+    </row>
+    <row r="38" spans="1:8" ht="48.75" customHeight="1">
+      <c r="A38" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-    </row>
-    <row r="38" spans="1:8" ht="48.75" customHeight="1">
-      <c r="A38" s="45" t="s">
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1929,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="15"/>
@@ -1951,70 +1933,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
     </row>
     <row r="6" spans="1:7" ht="83.25" customHeight="1">
-      <c r="A6" s="73" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
+      <c r="A6" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="5"/>
@@ -2023,51 +2005,51 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="35" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>7</v>
+        <v>54</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="32">
-        <v>45801</v>
+        <v>56</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="22.5" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.25" customHeight="1">
@@ -2089,168 +2071,163 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="25.5" customHeight="1">
-      <c r="B13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
+      <c r="A13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="25.5" customHeight="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" ht="24" customHeight="1">
+      <c r="A16" s="16"/>
+      <c r="B16" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="16" t="s">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="26.1" customHeight="1">
+      <c r="A17" s="16"/>
+      <c r="B17" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:7" ht="24" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="16" t="s">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="27.75" customHeight="1">
+      <c r="A18" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="27.75" customHeight="1">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" ht="27.75" customHeight="1">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" ht="42" customHeight="1">
+      <c r="A21" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="35"/>
+    </row>
+    <row r="22" spans="1:7" ht="61.5" customHeight="1">
+      <c r="A22" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="27.75" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-    </row>
-    <row r="21" spans="1:7" ht="27.75" customHeight="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" ht="42" customHeight="1">
-      <c r="A22" s="75" t="s">
+      <c r="B22" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
+      <c r="C22" s="73"/>
       <c r="D22" s="22"/>
-      <c r="E22" s="5"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="38"/>
-    </row>
-    <row r="23" spans="1:7" ht="61.5" customHeight="1">
-      <c r="A23" s="23" t="s">
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="33.950000000000003" customHeight="1">
+      <c r="A23" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A24" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" ht="33.950000000000003" customHeight="1">
-      <c r="A24" s="77" t="s">
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+    </row>
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A25" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A25" s="72" t="s">
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+    </row>
+    <row r="26" spans="1:7" ht="42" customHeight="1">
+      <c r="E26" s="31"/>
+      <c r="F26" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="24" customHeight="1">
+      <c r="E27" s="5"/>
+      <c r="F27" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-    </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1">
-      <c r="A26" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-    </row>
-    <row r="27" spans="1:7" ht="42" customHeight="1">
-      <c r="E27" s="34"/>
-      <c r="F27" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="24" customHeight="1">
+    </row>
+    <row r="28" spans="1:7" ht="69.75" customHeight="1">
       <c r="E28" s="5"/>
-      <c r="F28" s="27" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="69.75" customHeight="1">
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" ht="42" customHeight="1">
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:7" ht="42" customHeight="1">
+    <row r="30" spans="1:7" ht="53.1" customHeight="1">
       <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" ht="53.1" customHeight="1">
-      <c r="E31" s="5"/>
-      <c r="F31" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="G31" s="6"/>
-    </row>
+      <c r="F30" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" ht="27.75" customHeight="1"/>
     <row r="32" spans="1:7" ht="27.75" customHeight="1"/>
     <row r="33" ht="27.75" customHeight="1"/>
-    <row r="34" ht="27.75" customHeight="1"/>
-    <row r="35" ht="24.75" customHeight="1"/>
+    <row r="34" ht="24.75" customHeight="1"/>
+    <row r="35" ht="21" customHeight="1"/>
     <row r="36" ht="21" customHeight="1"/>
     <row r="37" ht="21" customHeight="1"/>
     <row r="38" ht="21" customHeight="1"/>
@@ -2258,31 +2235,30 @@
     <row r="40" ht="21" customHeight="1"/>
     <row r="41" ht="21" customHeight="1"/>
     <row r="42" ht="21" customHeight="1"/>
-    <row r="43" ht="21" customHeight="1"/>
-    <row r="44" ht="25.5" customHeight="1"/>
+    <row r="43" ht="25.5" customHeight="1"/>
+    <row r="44" ht="21" customHeight="1"/>
     <row r="45" ht="21" customHeight="1"/>
     <row r="46" ht="21" customHeight="1"/>
     <row r="47" ht="21" customHeight="1"/>
     <row r="48" ht="21" customHeight="1"/>
-    <row r="49" ht="21" customHeight="1"/>
-    <row r="50" ht="17.25" customHeight="1"/>
-    <row r="62" ht="15" customHeight="1"/>
+    <row r="49" ht="17.25" customHeight="1"/>
+    <row r="61" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A24:G24"/>
     <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A26:G26"/>
     <mergeCell ref="A6:G6"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
-  <conditionalFormatting sqref="J22:J34">
+  <conditionalFormatting sqref="J21:J33">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
     <cfRule type="uniqueValues" priority="2" stopIfTrue="1"/>
   </conditionalFormatting>
@@ -2294,10 +2270,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="15"/>
@@ -2317,94 +2293,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" ht="24" customHeight="1">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" spans="1:11" ht="54" customHeight="1">
-      <c r="A6" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
+      <c r="A6" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
     </row>
     <row r="7" spans="1:11" ht="14.25" customHeight="1">
       <c r="A7" s="5"/>
@@ -2415,56 +2391,56 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="80" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="80"/>
-      <c r="I8" s="31" t="s">
-        <v>7</v>
+      <c r="G8" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="77"/>
+      <c r="I8" s="28" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="32">
-        <v>45801</v>
+        <v>56</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="22.5" customHeight="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="34"/>
+        <v>58</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="20.25" customHeight="1">
       <c r="A11" s="5"/>
@@ -2492,62 +2468,66 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="25.5" customHeight="1">
-      <c r="B13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
+      <c r="A13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="3"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="3"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="25.5" customHeight="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="74" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="13"/>
+      <c r="B15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="3"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
+    <row r="16" spans="1:11" ht="24" customHeight="1">
+      <c r="A16" s="16"/>
+      <c r="B16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="24" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="16" t="s">
-        <v>66</v>
+    <row r="17" spans="1:12" ht="26.1" customHeight="1">
+      <c r="A17" s="16"/>
+      <c r="B17" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="26.1" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="16" t="s">
+    <row r="18" spans="1:12" ht="27.75" customHeight="1">
+      <c r="A18" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F18" s="3"/>
@@ -2555,148 +2535,138 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="27.75" customHeight="1">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="1:12" ht="27.75" customHeight="1">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="11"/>
+      <c r="L20" s="78"/>
+    </row>
+    <row r="21" spans="1:12" ht="48" customHeight="1">
+      <c r="A21" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="78"/>
+    </row>
+    <row r="22" spans="1:12" ht="72" customHeight="1">
+      <c r="A22" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" ht="27.75" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-    </row>
-    <row r="21" spans="1:12" ht="27.75" customHeight="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="13"/>
-      <c r="L21" s="81"/>
-    </row>
-    <row r="22" spans="1:12" ht="48" customHeight="1">
-      <c r="A22" s="75" t="s">
+      <c r="B22" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
+      <c r="C22" s="73"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
       <c r="H22" s="5"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="81"/>
-    </row>
-    <row r="23" spans="1:12" ht="72" customHeight="1">
-      <c r="A23" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="76" t="s">
+      <c r="L22" s="10"/>
+    </row>
+    <row r="23" spans="1:12" ht="42" customHeight="1">
+      <c r="A23" s="74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="10"/>
+    </row>
+    <row r="24" spans="1:12" ht="48" customHeight="1">
+      <c r="A24" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="10"/>
-    </row>
-    <row r="24" spans="1:12" ht="42" customHeight="1">
-      <c r="A24" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="10"/>
-    </row>
-    <row r="25" spans="1:12" ht="48" customHeight="1">
-      <c r="A25" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="72"/>
-    </row>
-    <row r="26" spans="1:12" s="1" customFormat="1" ht="48" customHeight="1">
-      <c r="A26" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
-    </row>
-    <row r="27" spans="1:12" ht="42" customHeight="1">
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+    </row>
+    <row r="25" spans="1:12" s="1" customFormat="1" ht="48" customHeight="1">
+      <c r="A25" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:12" ht="42" customHeight="1">
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" ht="24" customHeight="1">
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:12" ht="24" customHeight="1">
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="1:12" ht="69.75" customHeight="1">
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="27"/>
-    </row>
-    <row r="29" spans="1:12" ht="69.75" customHeight="1">
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:12" ht="42" customHeight="1">
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:12" ht="42" customHeight="1">
+      <c r="J29" s="76"/>
+      <c r="K29" s="76"/>
+    </row>
+    <row r="30" spans="1:12" ht="53.1" customHeight="1">
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="J30" s="79"/>
-      <c r="K30" s="79"/>
-    </row>
-    <row r="31" spans="1:12" ht="53.1" customHeight="1">
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-    </row>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" ht="27.75" customHeight="1"/>
     <row r="32" spans="1:12" ht="27.75" customHeight="1"/>
     <row r="33" ht="27.75" customHeight="1"/>
-    <row r="34" ht="27.75" customHeight="1"/>
-    <row r="35" ht="24.75" customHeight="1"/>
+    <row r="34" ht="24.75" customHeight="1"/>
+    <row r="35" ht="21" customHeight="1"/>
     <row r="36" ht="21" customHeight="1"/>
     <row r="37" ht="21" customHeight="1"/>
     <row r="38" ht="21" customHeight="1"/>
@@ -2704,34 +2674,33 @@
     <row r="40" ht="21" customHeight="1"/>
     <row r="41" ht="21" customHeight="1"/>
     <row r="42" ht="21" customHeight="1"/>
-    <row r="43" ht="21" customHeight="1"/>
-    <row r="44" ht="25.5" customHeight="1"/>
+    <row r="43" ht="25.5" customHeight="1"/>
+    <row r="44" ht="21" customHeight="1"/>
     <row r="45" ht="21" customHeight="1"/>
     <row r="46" ht="21" customHeight="1"/>
     <row r="47" ht="21" customHeight="1"/>
     <row r="48" ht="21" customHeight="1"/>
-    <row r="49" ht="21" customHeight="1"/>
-    <row r="50" ht="17.25" customHeight="1"/>
-    <row r="62" ht="15" customHeight="1"/>
+    <row r="49" ht="17.25" customHeight="1"/>
+    <row r="61" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:K24"/>
     <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J29:K29"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A5:I5"/>
   </mergeCells>
-  <conditionalFormatting sqref="N22:N34">
+  <conditionalFormatting sqref="N21:N33">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
     <cfRule type="uniqueValues" priority="2" stopIfTrue="1"/>
   </conditionalFormatting>

</xml_diff>